<commit_message>
Modified classes of the CANetwork to give the possibility to represent stairs. The behavior of agents inside stairs is the same, but they are updated once every two steps, thus with a speed of 0.65 m/s.
Modified and introduced .csv for the ABMUS paper.

The CASimulationRunner now contains some ad hoc code for this scenario,
that must be commented for different simulations.
</commit_message>
<xml_diff>
--- a/playgrounds/lcrociani/src/main/resources/visualizer.xlsx
+++ b/playgrounds/lcrociani/src/main/resources/visualizer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\workspace\playgrounds\lcrociani\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\git\matsim-org\matsim\playgrounds\lcrociani\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,8 @@
     <sheet name="environmentGrid" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ABMUS_PG_station2" localSheetId="0">environmentGrid!$A$1:$OS$103</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">environmentGrid!$A$1:$IR$103</definedName>
+    <definedName name="ABMUS_PG_station_separated" localSheetId="0">environmentGrid!$A$1:$IR$103</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -23,166 +24,9 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="ABMUS_PG_station2" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="850" sourceFile="C:\Users\Luca\workspace\playgrounds\lcrociani\src\main\resources\ABMUS_PG_station2.csv" thousands="'" semicolon="1">
-      <textFields count="409">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
+  <connection id="1" name="ABMUS_PG_station_separated" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\Luca\git\matsim-org\matsim\playgrounds\lcrociani\src\main\resources\ABMUS_PG_station_separated.csv" thousands="'" semicolon="1">
+      <textFields count="252">
         <textField/>
         <textField/>
         <textField/>
@@ -969,7 +813,56 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1026,7 +919,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ABMUS_PG_station2" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ABMUS_PG_station_separated" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1318,8 +1211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:OS103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AA14" sqref="AA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1386,7 +1279,7 @@
         <v>0</v>
       </c>
       <c r="S1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="T1">
         <v>-1</v>
@@ -2144,7 +2037,7 @@
         <v>0</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="T2">
         <v>0</v>
@@ -2156,7 +2049,7 @@
         <v>0</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="X2">
         <v>0</v>
@@ -2902,7 +2795,7 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -2914,7 +2807,7 @@
         <v>0</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="X3">
         <v>0</v>
@@ -3660,7 +3553,7 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="T4">
         <v>0</v>
@@ -3672,7 +3565,7 @@
         <v>0</v>
       </c>
       <c r="W4">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="X4">
         <v>0</v>
@@ -4418,7 +4311,7 @@
         <v>0</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="T5">
         <v>0</v>
@@ -4430,7 +4323,7 @@
         <v>0</v>
       </c>
       <c r="W5">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="X5">
         <v>0</v>
@@ -5176,7 +5069,7 @@
         <v>0</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -5188,7 +5081,7 @@
         <v>0</v>
       </c>
       <c r="W6">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="X6">
         <v>0</v>
@@ -5934,7 +5827,7 @@
         <v>0</v>
       </c>
       <c r="S7">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="T7">
         <v>0</v>
@@ -5946,7 +5839,7 @@
         <v>0</v>
       </c>
       <c r="W7">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="X7">
         <v>0</v>
@@ -6692,7 +6585,7 @@
         <v>0</v>
       </c>
       <c r="S8">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="T8">
         <v>0</v>
@@ -6704,7 +6597,7 @@
         <v>0</v>
       </c>
       <c r="W8">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="X8">
         <v>0</v>
@@ -7450,7 +7343,7 @@
         <v>0</v>
       </c>
       <c r="S9">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="T9">
         <v>0</v>
@@ -7462,7 +7355,7 @@
         <v>0</v>
       </c>
       <c r="W9">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="X9">
         <v>0</v>
@@ -8209,7 +8102,7 @@
         <v>0</v>
       </c>
       <c r="S10">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="T10">
         <v>0</v>
@@ -8221,7 +8114,7 @@
         <v>0</v>
       </c>
       <c r="W10">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="X10">
         <v>0</v>
@@ -8967,7 +8860,7 @@
         <v>0</v>
       </c>
       <c r="S11">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="T11">
         <v>0</v>
@@ -8979,7 +8872,7 @@
         <v>0</v>
       </c>
       <c r="W11">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="X11">
         <v>0</v>
@@ -9725,7 +9618,7 @@
         <v>0</v>
       </c>
       <c r="S12">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="T12">
         <v>0</v>
@@ -9737,7 +9630,7 @@
         <v>0</v>
       </c>
       <c r="W12">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="X12">
         <v>0</v>
@@ -10483,7 +10376,7 @@
         <v>0</v>
       </c>
       <c r="S13">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="T13">
         <v>0</v>
@@ -10495,7 +10388,7 @@
         <v>0</v>
       </c>
       <c r="W13">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="X13">
         <v>0</v>
@@ -11241,28 +11134,28 @@
         <v>0</v>
       </c>
       <c r="S14">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="T14">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="U14">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="V14">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="W14">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X14">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="Y14">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="Z14">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="AA14">
         <v>-1</v>
@@ -11999,7 +11892,7 @@
         <v>0</v>
       </c>
       <c r="S15">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="T15">
         <v>0</v>
@@ -12011,7 +11904,7 @@
         <v>0</v>
       </c>
       <c r="W15">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="X15">
         <v>0</v>
@@ -12757,7 +12650,7 @@
         <v>0</v>
       </c>
       <c r="S16">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="T16">
         <v>0</v>
@@ -12769,7 +12662,7 @@
         <v>0</v>
       </c>
       <c r="W16">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="X16">
         <v>0</v>
@@ -13515,7 +13408,7 @@
         <v>0</v>
       </c>
       <c r="S17">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="T17">
         <v>0</v>
@@ -13527,7 +13420,7 @@
         <v>0</v>
       </c>
       <c r="W17">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="X17">
         <v>0</v>
@@ -14273,7 +14166,7 @@
         <v>0</v>
       </c>
       <c r="S18">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="T18">
         <v>0</v>
@@ -14285,7 +14178,7 @@
         <v>0</v>
       </c>
       <c r="W18">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="X18">
         <v>0</v>
@@ -15031,7 +14924,7 @@
         <v>0</v>
       </c>
       <c r="S19">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="T19">
         <v>0</v>
@@ -15043,7 +14936,7 @@
         <v>0</v>
       </c>
       <c r="W19">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="X19">
         <v>0</v>
@@ -15792,25 +15685,25 @@
         <v>-2</v>
       </c>
       <c r="T20">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="U20">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="V20">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="W20">
         <v>-2</v>
       </c>
       <c r="X20">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="Y20">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="Z20">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="AA20">
         <v>-1</v>
@@ -16550,25 +16443,25 @@
         <v>-1</v>
       </c>
       <c r="T21">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="U21">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="V21">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="W21">
         <v>-1</v>
       </c>
       <c r="X21">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="Y21">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="Z21">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="AA21">
         <v>-1</v>
@@ -25293,7 +25186,7 @@
         <v>0</v>
       </c>
       <c r="EY32">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="EZ32">
         <v>0</v>
@@ -26051,7 +25944,7 @@
         <v>0</v>
       </c>
       <c r="EY33">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="EZ33">
         <v>0</v>
@@ -26809,7 +26702,7 @@
         <v>0</v>
       </c>
       <c r="EY34">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="EZ34">
         <v>0</v>
@@ -27567,7 +27460,7 @@
         <v>0</v>
       </c>
       <c r="EY35">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="EZ35">
         <v>0</v>
@@ -28325,7 +28218,7 @@
         <v>0</v>
       </c>
       <c r="EY36">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="EZ36">
         <v>0</v>
@@ -29083,7 +28976,7 @@
         <v>0</v>
       </c>
       <c r="EY37">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="EZ37">
         <v>0</v>
@@ -29841,7 +29734,7 @@
         <v>0</v>
       </c>
       <c r="EY38">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="EZ38">
         <v>0</v>
@@ -30599,7 +30492,7 @@
         <v>0</v>
       </c>
       <c r="EY39">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="EZ39">
         <v>0</v>
@@ -31357,7 +31250,7 @@
         <v>0</v>
       </c>
       <c r="EY40">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="EZ40">
         <v>0</v>
@@ -32115,7 +32008,7 @@
         <v>0</v>
       </c>
       <c r="EY41">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="EZ41">
         <v>0</v>
@@ -32873,7 +32766,7 @@
         <v>0</v>
       </c>
       <c r="EY42">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="EZ42">
         <v>0</v>
@@ -33631,7 +33524,7 @@
         <v>0</v>
       </c>
       <c r="EY43">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="EZ43">
         <v>0</v>
@@ -34389,7 +34282,7 @@
         <v>0</v>
       </c>
       <c r="EY44">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="EZ44">
         <v>0</v>
@@ -35147,7 +35040,7 @@
         <v>0</v>
       </c>
       <c r="EY45">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="EZ45">
         <v>0</v>
@@ -35905,7 +35798,7 @@
         <v>0</v>
       </c>
       <c r="EY46">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="EZ46">
         <v>0</v>
@@ -36663,7 +36556,7 @@
         <v>0</v>
       </c>
       <c r="EY47">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="EZ47">
         <v>0</v>
@@ -37421,7 +37314,7 @@
         <v>0</v>
       </c>
       <c r="EY48">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="EZ48">
         <v>0</v>
@@ -38179,7 +38072,7 @@
         <v>0</v>
       </c>
       <c r="EY49">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="EZ49">
         <v>0</v>
@@ -38937,7 +38830,7 @@
         <v>0</v>
       </c>
       <c r="EY50">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="EZ50">
         <v>0</v>
@@ -39290,412 +39183,412 @@
         <v>-1</v>
       </c>
       <c r="T51">
+        <v>-4</v>
+      </c>
+      <c r="U51">
+        <v>-4</v>
+      </c>
+      <c r="V51">
+        <v>-4</v>
+      </c>
+      <c r="W51">
+        <v>-1</v>
+      </c>
+      <c r="X51">
+        <v>-4</v>
+      </c>
+      <c r="Y51">
+        <v>-4</v>
+      </c>
+      <c r="Z51">
+        <v>-4</v>
+      </c>
+      <c r="AA51">
+        <v>-1</v>
+      </c>
+      <c r="AB51">
+        <v>-1</v>
+      </c>
+      <c r="AC51">
+        <v>-1</v>
+      </c>
+      <c r="AD51">
+        <v>-1</v>
+      </c>
+      <c r="AE51">
+        <v>-1</v>
+      </c>
+      <c r="AF51">
+        <v>-1</v>
+      </c>
+      <c r="AG51">
+        <v>-1</v>
+      </c>
+      <c r="AH51">
+        <v>-1</v>
+      </c>
+      <c r="AI51">
+        <v>-1</v>
+      </c>
+      <c r="AJ51">
+        <v>-1</v>
+      </c>
+      <c r="AK51">
+        <v>-1</v>
+      </c>
+      <c r="AL51">
+        <v>-1</v>
+      </c>
+      <c r="AM51">
+        <v>-1</v>
+      </c>
+      <c r="AN51">
+        <v>-1</v>
+      </c>
+      <c r="AO51">
+        <v>-1</v>
+      </c>
+      <c r="AP51">
+        <v>-1</v>
+      </c>
+      <c r="AQ51">
+        <v>-1</v>
+      </c>
+      <c r="AR51">
+        <v>-1</v>
+      </c>
+      <c r="AS51">
+        <v>-1</v>
+      </c>
+      <c r="AT51">
+        <v>-1</v>
+      </c>
+      <c r="AU51">
+        <v>-1</v>
+      </c>
+      <c r="AV51">
+        <v>-1</v>
+      </c>
+      <c r="AW51">
+        <v>-1</v>
+      </c>
+      <c r="AX51">
+        <v>-1</v>
+      </c>
+      <c r="AY51">
+        <v>-1</v>
+      </c>
+      <c r="AZ51">
+        <v>-1</v>
+      </c>
+      <c r="BA51">
+        <v>-1</v>
+      </c>
+      <c r="BB51">
+        <v>-1</v>
+      </c>
+      <c r="BC51">
+        <v>-1</v>
+      </c>
+      <c r="BD51">
+        <v>-1</v>
+      </c>
+      <c r="BE51">
+        <v>-1</v>
+      </c>
+      <c r="BF51">
+        <v>-1</v>
+      </c>
+      <c r="BG51">
+        <v>-1</v>
+      </c>
+      <c r="BH51">
+        <v>-1</v>
+      </c>
+      <c r="BI51">
+        <v>-1</v>
+      </c>
+      <c r="BJ51">
+        <v>-1</v>
+      </c>
+      <c r="BK51">
+        <v>-1</v>
+      </c>
+      <c r="BL51">
+        <v>-1</v>
+      </c>
+      <c r="BM51">
+        <v>-1</v>
+      </c>
+      <c r="BN51">
+        <v>-1</v>
+      </c>
+      <c r="BO51">
+        <v>-1</v>
+      </c>
+      <c r="BP51">
+        <v>-1</v>
+      </c>
+      <c r="BQ51">
+        <v>-1</v>
+      </c>
+      <c r="BR51">
+        <v>-1</v>
+      </c>
+      <c r="BS51">
+        <v>-1</v>
+      </c>
+      <c r="BT51">
+        <v>-1</v>
+      </c>
+      <c r="BU51">
+        <v>-1</v>
+      </c>
+      <c r="BV51">
+        <v>-1</v>
+      </c>
+      <c r="BW51">
+        <v>-1</v>
+      </c>
+      <c r="BX51">
+        <v>-1</v>
+      </c>
+      <c r="BY51">
+        <v>-1</v>
+      </c>
+      <c r="BZ51">
+        <v>-1</v>
+      </c>
+      <c r="CA51">
+        <v>-1</v>
+      </c>
+      <c r="CB51">
+        <v>-1</v>
+      </c>
+      <c r="CC51">
+        <v>-1</v>
+      </c>
+      <c r="CD51">
+        <v>-1</v>
+      </c>
+      <c r="CE51">
+        <v>-1</v>
+      </c>
+      <c r="CF51">
+        <v>-1</v>
+      </c>
+      <c r="CG51">
+        <v>-1</v>
+      </c>
+      <c r="CH51">
+        <v>-1</v>
+      </c>
+      <c r="CI51">
+        <v>-1</v>
+      </c>
+      <c r="CJ51">
+        <v>-1</v>
+      </c>
+      <c r="CK51">
+        <v>-1</v>
+      </c>
+      <c r="CL51">
+        <v>-1</v>
+      </c>
+      <c r="CM51">
+        <v>-1</v>
+      </c>
+      <c r="CN51">
+        <v>-1</v>
+      </c>
+      <c r="CO51">
+        <v>-1</v>
+      </c>
+      <c r="CP51">
+        <v>-1</v>
+      </c>
+      <c r="CQ51">
+        <v>-1</v>
+      </c>
+      <c r="CR51">
+        <v>-1</v>
+      </c>
+      <c r="CS51">
+        <v>-1</v>
+      </c>
+      <c r="CT51">
+        <v>-1</v>
+      </c>
+      <c r="CU51">
+        <v>-1</v>
+      </c>
+      <c r="CV51">
+        <v>-1</v>
+      </c>
+      <c r="CW51">
+        <v>-1</v>
+      </c>
+      <c r="CX51">
+        <v>-1</v>
+      </c>
+      <c r="CY51">
+        <v>-1</v>
+      </c>
+      <c r="CZ51">
+        <v>-1</v>
+      </c>
+      <c r="DA51">
+        <v>-1</v>
+      </c>
+      <c r="DB51">
+        <v>-1</v>
+      </c>
+      <c r="DC51">
+        <v>-1</v>
+      </c>
+      <c r="DD51">
+        <v>-1</v>
+      </c>
+      <c r="DE51">
+        <v>-1</v>
+      </c>
+      <c r="DF51">
+        <v>-1</v>
+      </c>
+      <c r="DG51">
+        <v>-1</v>
+      </c>
+      <c r="DH51">
+        <v>-1</v>
+      </c>
+      <c r="DI51">
+        <v>-1</v>
+      </c>
+      <c r="DJ51">
+        <v>-1</v>
+      </c>
+      <c r="DK51">
+        <v>-1</v>
+      </c>
+      <c r="DL51">
+        <v>-1</v>
+      </c>
+      <c r="DM51">
+        <v>-1</v>
+      </c>
+      <c r="DN51">
+        <v>-1</v>
+      </c>
+      <c r="DO51">
+        <v>-1</v>
+      </c>
+      <c r="DP51">
+        <v>-1</v>
+      </c>
+      <c r="DQ51">
+        <v>-1</v>
+      </c>
+      <c r="DR51">
+        <v>-1</v>
+      </c>
+      <c r="DS51">
+        <v>-1</v>
+      </c>
+      <c r="DT51">
+        <v>-1</v>
+      </c>
+      <c r="DU51">
+        <v>-1</v>
+      </c>
+      <c r="DV51">
+        <v>-1</v>
+      </c>
+      <c r="DW51">
+        <v>-1</v>
+      </c>
+      <c r="DX51">
+        <v>-1</v>
+      </c>
+      <c r="DY51">
+        <v>-1</v>
+      </c>
+      <c r="DZ51">
+        <v>-1</v>
+      </c>
+      <c r="EA51">
+        <v>-1</v>
+      </c>
+      <c r="EB51">
+        <v>-1</v>
+      </c>
+      <c r="EC51">
+        <v>-1</v>
+      </c>
+      <c r="ED51">
+        <v>-1</v>
+      </c>
+      <c r="EE51">
+        <v>-1</v>
+      </c>
+      <c r="EF51">
+        <v>-1</v>
+      </c>
+      <c r="EG51">
+        <v>-1</v>
+      </c>
+      <c r="EH51">
+        <v>-1</v>
+      </c>
+      <c r="EI51">
+        <v>-1</v>
+      </c>
+      <c r="EJ51">
+        <v>-1</v>
+      </c>
+      <c r="EK51">
+        <v>-1</v>
+      </c>
+      <c r="EL51">
+        <v>-1</v>
+      </c>
+      <c r="EM51">
+        <v>-1</v>
+      </c>
+      <c r="EN51">
+        <v>-1</v>
+      </c>
+      <c r="EO51">
+        <v>0</v>
+      </c>
+      <c r="EP51">
+        <v>0</v>
+      </c>
+      <c r="EQ51">
+        <v>0</v>
+      </c>
+      <c r="ER51">
+        <v>0</v>
+      </c>
+      <c r="ES51">
+        <v>0</v>
+      </c>
+      <c r="ET51">
+        <v>0</v>
+      </c>
+      <c r="EU51">
+        <v>0</v>
+      </c>
+      <c r="EV51">
+        <v>0</v>
+      </c>
+      <c r="EW51">
+        <v>0</v>
+      </c>
+      <c r="EX51">
+        <v>0</v>
+      </c>
+      <c r="EY51">
         <v>-2</v>
-      </c>
-      <c r="U51">
-        <v>-2</v>
-      </c>
-      <c r="V51">
-        <v>-2</v>
-      </c>
-      <c r="W51">
-        <v>-1</v>
-      </c>
-      <c r="X51">
-        <v>-2</v>
-      </c>
-      <c r="Y51">
-        <v>-2</v>
-      </c>
-      <c r="Z51">
-        <v>-2</v>
-      </c>
-      <c r="AA51">
-        <v>-1</v>
-      </c>
-      <c r="AB51">
-        <v>-1</v>
-      </c>
-      <c r="AC51">
-        <v>-1</v>
-      </c>
-      <c r="AD51">
-        <v>-1</v>
-      </c>
-      <c r="AE51">
-        <v>-1</v>
-      </c>
-      <c r="AF51">
-        <v>-1</v>
-      </c>
-      <c r="AG51">
-        <v>-1</v>
-      </c>
-      <c r="AH51">
-        <v>-1</v>
-      </c>
-      <c r="AI51">
-        <v>-1</v>
-      </c>
-      <c r="AJ51">
-        <v>-1</v>
-      </c>
-      <c r="AK51">
-        <v>-1</v>
-      </c>
-      <c r="AL51">
-        <v>-1</v>
-      </c>
-      <c r="AM51">
-        <v>-1</v>
-      </c>
-      <c r="AN51">
-        <v>-1</v>
-      </c>
-      <c r="AO51">
-        <v>-1</v>
-      </c>
-      <c r="AP51">
-        <v>-1</v>
-      </c>
-      <c r="AQ51">
-        <v>-1</v>
-      </c>
-      <c r="AR51">
-        <v>-1</v>
-      </c>
-      <c r="AS51">
-        <v>-1</v>
-      </c>
-      <c r="AT51">
-        <v>-1</v>
-      </c>
-      <c r="AU51">
-        <v>-1</v>
-      </c>
-      <c r="AV51">
-        <v>-1</v>
-      </c>
-      <c r="AW51">
-        <v>-1</v>
-      </c>
-      <c r="AX51">
-        <v>-1</v>
-      </c>
-      <c r="AY51">
-        <v>-1</v>
-      </c>
-      <c r="AZ51">
-        <v>-1</v>
-      </c>
-      <c r="BA51">
-        <v>-1</v>
-      </c>
-      <c r="BB51">
-        <v>-1</v>
-      </c>
-      <c r="BC51">
-        <v>-1</v>
-      </c>
-      <c r="BD51">
-        <v>-1</v>
-      </c>
-      <c r="BE51">
-        <v>-1</v>
-      </c>
-      <c r="BF51">
-        <v>-1</v>
-      </c>
-      <c r="BG51">
-        <v>-1</v>
-      </c>
-      <c r="BH51">
-        <v>-1</v>
-      </c>
-      <c r="BI51">
-        <v>-1</v>
-      </c>
-      <c r="BJ51">
-        <v>-1</v>
-      </c>
-      <c r="BK51">
-        <v>-1</v>
-      </c>
-      <c r="BL51">
-        <v>-1</v>
-      </c>
-      <c r="BM51">
-        <v>-1</v>
-      </c>
-      <c r="BN51">
-        <v>-1</v>
-      </c>
-      <c r="BO51">
-        <v>-1</v>
-      </c>
-      <c r="BP51">
-        <v>-1</v>
-      </c>
-      <c r="BQ51">
-        <v>-1</v>
-      </c>
-      <c r="BR51">
-        <v>-1</v>
-      </c>
-      <c r="BS51">
-        <v>-1</v>
-      </c>
-      <c r="BT51">
-        <v>-1</v>
-      </c>
-      <c r="BU51">
-        <v>-1</v>
-      </c>
-      <c r="BV51">
-        <v>-1</v>
-      </c>
-      <c r="BW51">
-        <v>-1</v>
-      </c>
-      <c r="BX51">
-        <v>-1</v>
-      </c>
-      <c r="BY51">
-        <v>-1</v>
-      </c>
-      <c r="BZ51">
-        <v>-1</v>
-      </c>
-      <c r="CA51">
-        <v>-1</v>
-      </c>
-      <c r="CB51">
-        <v>-1</v>
-      </c>
-      <c r="CC51">
-        <v>-1</v>
-      </c>
-      <c r="CD51">
-        <v>-1</v>
-      </c>
-      <c r="CE51">
-        <v>-1</v>
-      </c>
-      <c r="CF51">
-        <v>-1</v>
-      </c>
-      <c r="CG51">
-        <v>-1</v>
-      </c>
-      <c r="CH51">
-        <v>-1</v>
-      </c>
-      <c r="CI51">
-        <v>-1</v>
-      </c>
-      <c r="CJ51">
-        <v>-1</v>
-      </c>
-      <c r="CK51">
-        <v>-1</v>
-      </c>
-      <c r="CL51">
-        <v>-1</v>
-      </c>
-      <c r="CM51">
-        <v>-1</v>
-      </c>
-      <c r="CN51">
-        <v>-1</v>
-      </c>
-      <c r="CO51">
-        <v>-1</v>
-      </c>
-      <c r="CP51">
-        <v>-1</v>
-      </c>
-      <c r="CQ51">
-        <v>-1</v>
-      </c>
-      <c r="CR51">
-        <v>-1</v>
-      </c>
-      <c r="CS51">
-        <v>-1</v>
-      </c>
-      <c r="CT51">
-        <v>-1</v>
-      </c>
-      <c r="CU51">
-        <v>-1</v>
-      </c>
-      <c r="CV51">
-        <v>-1</v>
-      </c>
-      <c r="CW51">
-        <v>-1</v>
-      </c>
-      <c r="CX51">
-        <v>-1</v>
-      </c>
-      <c r="CY51">
-        <v>-1</v>
-      </c>
-      <c r="CZ51">
-        <v>-1</v>
-      </c>
-      <c r="DA51">
-        <v>-1</v>
-      </c>
-      <c r="DB51">
-        <v>-1</v>
-      </c>
-      <c r="DC51">
-        <v>-1</v>
-      </c>
-      <c r="DD51">
-        <v>-1</v>
-      </c>
-      <c r="DE51">
-        <v>-1</v>
-      </c>
-      <c r="DF51">
-        <v>-1</v>
-      </c>
-      <c r="DG51">
-        <v>-1</v>
-      </c>
-      <c r="DH51">
-        <v>-1</v>
-      </c>
-      <c r="DI51">
-        <v>-1</v>
-      </c>
-      <c r="DJ51">
-        <v>-1</v>
-      </c>
-      <c r="DK51">
-        <v>-1</v>
-      </c>
-      <c r="DL51">
-        <v>-1</v>
-      </c>
-      <c r="DM51">
-        <v>-1</v>
-      </c>
-      <c r="DN51">
-        <v>-1</v>
-      </c>
-      <c r="DO51">
-        <v>-1</v>
-      </c>
-      <c r="DP51">
-        <v>-1</v>
-      </c>
-      <c r="DQ51">
-        <v>-1</v>
-      </c>
-      <c r="DR51">
-        <v>-1</v>
-      </c>
-      <c r="DS51">
-        <v>-1</v>
-      </c>
-      <c r="DT51">
-        <v>-1</v>
-      </c>
-      <c r="DU51">
-        <v>-1</v>
-      </c>
-      <c r="DV51">
-        <v>-1</v>
-      </c>
-      <c r="DW51">
-        <v>-1</v>
-      </c>
-      <c r="DX51">
-        <v>-1</v>
-      </c>
-      <c r="DY51">
-        <v>-1</v>
-      </c>
-      <c r="DZ51">
-        <v>-1</v>
-      </c>
-      <c r="EA51">
-        <v>-1</v>
-      </c>
-      <c r="EB51">
-        <v>-1</v>
-      </c>
-      <c r="EC51">
-        <v>-1</v>
-      </c>
-      <c r="ED51">
-        <v>-1</v>
-      </c>
-      <c r="EE51">
-        <v>-1</v>
-      </c>
-      <c r="EF51">
-        <v>-1</v>
-      </c>
-      <c r="EG51">
-        <v>-1</v>
-      </c>
-      <c r="EH51">
-        <v>-1</v>
-      </c>
-      <c r="EI51">
-        <v>-1</v>
-      </c>
-      <c r="EJ51">
-        <v>-1</v>
-      </c>
-      <c r="EK51">
-        <v>-1</v>
-      </c>
-      <c r="EL51">
-        <v>-1</v>
-      </c>
-      <c r="EM51">
-        <v>-1</v>
-      </c>
-      <c r="EN51">
-        <v>-1</v>
-      </c>
-      <c r="EO51">
-        <v>-2</v>
-      </c>
-      <c r="EP51">
-        <v>0</v>
-      </c>
-      <c r="EQ51">
-        <v>0</v>
-      </c>
-      <c r="ER51">
-        <v>0</v>
-      </c>
-      <c r="ES51">
-        <v>0</v>
-      </c>
-      <c r="ET51">
-        <v>0</v>
-      </c>
-      <c r="EU51">
-        <v>0</v>
-      </c>
-      <c r="EV51">
-        <v>0</v>
-      </c>
-      <c r="EW51">
-        <v>0</v>
-      </c>
-      <c r="EX51">
-        <v>0</v>
-      </c>
-      <c r="EY51">
-        <v>0</v>
       </c>
       <c r="EZ51">
         <v>0</v>
@@ -40057,7 +39950,7 @@
         <v>0</v>
       </c>
       <c r="W52">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X52">
         <v>0</v>
@@ -40300,160 +40193,160 @@
         <v>0</v>
       </c>
       <c r="CZ52">
+        <v>0</v>
+      </c>
+      <c r="DA52">
+        <v>0</v>
+      </c>
+      <c r="DB52">
+        <v>0</v>
+      </c>
+      <c r="DC52">
+        <v>0</v>
+      </c>
+      <c r="DD52">
+        <v>0</v>
+      </c>
+      <c r="DE52">
+        <v>0</v>
+      </c>
+      <c r="DF52">
+        <v>0</v>
+      </c>
+      <c r="DG52">
+        <v>0</v>
+      </c>
+      <c r="DH52">
+        <v>0</v>
+      </c>
+      <c r="DI52">
+        <v>0</v>
+      </c>
+      <c r="DJ52">
+        <v>-4</v>
+      </c>
+      <c r="DK52">
+        <v>0</v>
+      </c>
+      <c r="DL52">
+        <v>0</v>
+      </c>
+      <c r="DM52">
+        <v>0</v>
+      </c>
+      <c r="DN52">
+        <v>0</v>
+      </c>
+      <c r="DO52">
+        <v>0</v>
+      </c>
+      <c r="DP52">
+        <v>0</v>
+      </c>
+      <c r="DQ52">
+        <v>0</v>
+      </c>
+      <c r="DR52">
+        <v>0</v>
+      </c>
+      <c r="DS52">
+        <v>0</v>
+      </c>
+      <c r="DT52">
+        <v>0</v>
+      </c>
+      <c r="DU52">
+        <v>0</v>
+      </c>
+      <c r="DV52">
+        <v>0</v>
+      </c>
+      <c r="DW52">
+        <v>0</v>
+      </c>
+      <c r="DX52">
+        <v>0</v>
+      </c>
+      <c r="DY52">
+        <v>0</v>
+      </c>
+      <c r="DZ52">
+        <v>0</v>
+      </c>
+      <c r="EA52">
+        <v>0</v>
+      </c>
+      <c r="EB52">
+        <v>0</v>
+      </c>
+      <c r="EC52">
+        <v>0</v>
+      </c>
+      <c r="ED52">
+        <v>0</v>
+      </c>
+      <c r="EE52">
+        <v>0</v>
+      </c>
+      <c r="EF52">
+        <v>0</v>
+      </c>
+      <c r="EG52">
+        <v>0</v>
+      </c>
+      <c r="EH52">
+        <v>0</v>
+      </c>
+      <c r="EI52">
+        <v>0</v>
+      </c>
+      <c r="EJ52">
+        <v>0</v>
+      </c>
+      <c r="EK52">
+        <v>0</v>
+      </c>
+      <c r="EL52">
+        <v>0</v>
+      </c>
+      <c r="EM52">
+        <v>0</v>
+      </c>
+      <c r="EN52">
+        <v>-4</v>
+      </c>
+      <c r="EO52">
+        <v>0</v>
+      </c>
+      <c r="EP52">
+        <v>0</v>
+      </c>
+      <c r="EQ52">
+        <v>0</v>
+      </c>
+      <c r="ER52">
+        <v>0</v>
+      </c>
+      <c r="ES52">
+        <v>0</v>
+      </c>
+      <c r="ET52">
+        <v>0</v>
+      </c>
+      <c r="EU52">
+        <v>0</v>
+      </c>
+      <c r="EV52">
+        <v>0</v>
+      </c>
+      <c r="EW52">
+        <v>0</v>
+      </c>
+      <c r="EX52">
+        <v>0</v>
+      </c>
+      <c r="EY52">
         <v>-2</v>
-      </c>
-      <c r="DA52">
-        <v>0</v>
-      </c>
-      <c r="DB52">
-        <v>0</v>
-      </c>
-      <c r="DC52">
-        <v>0</v>
-      </c>
-      <c r="DD52">
-        <v>0</v>
-      </c>
-      <c r="DE52">
-        <v>0</v>
-      </c>
-      <c r="DF52">
-        <v>0</v>
-      </c>
-      <c r="DG52">
-        <v>0</v>
-      </c>
-      <c r="DH52">
-        <v>0</v>
-      </c>
-      <c r="DI52">
-        <v>0</v>
-      </c>
-      <c r="DJ52">
-        <v>0</v>
-      </c>
-      <c r="DK52">
-        <v>0</v>
-      </c>
-      <c r="DL52">
-        <v>0</v>
-      </c>
-      <c r="DM52">
-        <v>0</v>
-      </c>
-      <c r="DN52">
-        <v>0</v>
-      </c>
-      <c r="DO52">
-        <v>0</v>
-      </c>
-      <c r="DP52">
-        <v>0</v>
-      </c>
-      <c r="DQ52">
-        <v>0</v>
-      </c>
-      <c r="DR52">
-        <v>0</v>
-      </c>
-      <c r="DS52">
-        <v>0</v>
-      </c>
-      <c r="DT52">
-        <v>0</v>
-      </c>
-      <c r="DU52">
-        <v>0</v>
-      </c>
-      <c r="DV52">
-        <v>0</v>
-      </c>
-      <c r="DW52">
-        <v>0</v>
-      </c>
-      <c r="DX52">
-        <v>0</v>
-      </c>
-      <c r="DY52">
-        <v>0</v>
-      </c>
-      <c r="DZ52">
-        <v>0</v>
-      </c>
-      <c r="EA52">
-        <v>0</v>
-      </c>
-      <c r="EB52">
-        <v>0</v>
-      </c>
-      <c r="EC52">
-        <v>0</v>
-      </c>
-      <c r="ED52">
-        <v>0</v>
-      </c>
-      <c r="EE52">
-        <v>0</v>
-      </c>
-      <c r="EF52">
-        <v>0</v>
-      </c>
-      <c r="EG52">
-        <v>0</v>
-      </c>
-      <c r="EH52">
-        <v>0</v>
-      </c>
-      <c r="EI52">
-        <v>0</v>
-      </c>
-      <c r="EJ52">
-        <v>0</v>
-      </c>
-      <c r="EK52">
-        <v>0</v>
-      </c>
-      <c r="EL52">
-        <v>0</v>
-      </c>
-      <c r="EM52">
-        <v>0</v>
-      </c>
-      <c r="EN52">
-        <v>0</v>
-      </c>
-      <c r="EO52">
-        <v>-2</v>
-      </c>
-      <c r="EP52">
-        <v>0</v>
-      </c>
-      <c r="EQ52">
-        <v>0</v>
-      </c>
-      <c r="ER52">
-        <v>0</v>
-      </c>
-      <c r="ES52">
-        <v>0</v>
-      </c>
-      <c r="ET52">
-        <v>0</v>
-      </c>
-      <c r="EU52">
-        <v>0</v>
-      </c>
-      <c r="EV52">
-        <v>0</v>
-      </c>
-      <c r="EW52">
-        <v>0</v>
-      </c>
-      <c r="EX52">
-        <v>0</v>
-      </c>
-      <c r="EY52">
-        <v>0</v>
       </c>
       <c r="EZ52">
         <v>0</v>
@@ -40815,7 +40708,7 @@
         <v>0</v>
       </c>
       <c r="W53">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X53">
         <v>0</v>
@@ -41058,160 +40951,160 @@
         <v>0</v>
       </c>
       <c r="CZ53">
+        <v>0</v>
+      </c>
+      <c r="DA53">
+        <v>0</v>
+      </c>
+      <c r="DB53">
+        <v>0</v>
+      </c>
+      <c r="DC53">
+        <v>0</v>
+      </c>
+      <c r="DD53">
+        <v>0</v>
+      </c>
+      <c r="DE53">
+        <v>0</v>
+      </c>
+      <c r="DF53">
+        <v>0</v>
+      </c>
+      <c r="DG53">
+        <v>0</v>
+      </c>
+      <c r="DH53">
+        <v>0</v>
+      </c>
+      <c r="DI53">
+        <v>0</v>
+      </c>
+      <c r="DJ53">
+        <v>-4</v>
+      </c>
+      <c r="DK53">
+        <v>0</v>
+      </c>
+      <c r="DL53">
+        <v>0</v>
+      </c>
+      <c r="DM53">
+        <v>0</v>
+      </c>
+      <c r="DN53">
+        <v>0</v>
+      </c>
+      <c r="DO53">
+        <v>0</v>
+      </c>
+      <c r="DP53">
+        <v>0</v>
+      </c>
+      <c r="DQ53">
+        <v>0</v>
+      </c>
+      <c r="DR53">
+        <v>0</v>
+      </c>
+      <c r="DS53">
+        <v>0</v>
+      </c>
+      <c r="DT53">
+        <v>0</v>
+      </c>
+      <c r="DU53">
+        <v>0</v>
+      </c>
+      <c r="DV53">
+        <v>0</v>
+      </c>
+      <c r="DW53">
+        <v>0</v>
+      </c>
+      <c r="DX53">
+        <v>0</v>
+      </c>
+      <c r="DY53">
+        <v>0</v>
+      </c>
+      <c r="DZ53">
+        <v>0</v>
+      </c>
+      <c r="EA53">
+        <v>0</v>
+      </c>
+      <c r="EB53">
+        <v>0</v>
+      </c>
+      <c r="EC53">
+        <v>0</v>
+      </c>
+      <c r="ED53">
+        <v>0</v>
+      </c>
+      <c r="EE53">
+        <v>0</v>
+      </c>
+      <c r="EF53">
+        <v>0</v>
+      </c>
+      <c r="EG53">
+        <v>0</v>
+      </c>
+      <c r="EH53">
+        <v>0</v>
+      </c>
+      <c r="EI53">
+        <v>0</v>
+      </c>
+      <c r="EJ53">
+        <v>0</v>
+      </c>
+      <c r="EK53">
+        <v>0</v>
+      </c>
+      <c r="EL53">
+        <v>0</v>
+      </c>
+      <c r="EM53">
+        <v>0</v>
+      </c>
+      <c r="EN53">
+        <v>-4</v>
+      </c>
+      <c r="EO53">
+        <v>0</v>
+      </c>
+      <c r="EP53">
+        <v>0</v>
+      </c>
+      <c r="EQ53">
+        <v>0</v>
+      </c>
+      <c r="ER53">
+        <v>0</v>
+      </c>
+      <c r="ES53">
+        <v>0</v>
+      </c>
+      <c r="ET53">
+        <v>0</v>
+      </c>
+      <c r="EU53">
+        <v>0</v>
+      </c>
+      <c r="EV53">
+        <v>0</v>
+      </c>
+      <c r="EW53">
+        <v>0</v>
+      </c>
+      <c r="EX53">
+        <v>0</v>
+      </c>
+      <c r="EY53">
         <v>-2</v>
-      </c>
-      <c r="DA53">
-        <v>0</v>
-      </c>
-      <c r="DB53">
-        <v>0</v>
-      </c>
-      <c r="DC53">
-        <v>0</v>
-      </c>
-      <c r="DD53">
-        <v>0</v>
-      </c>
-      <c r="DE53">
-        <v>0</v>
-      </c>
-      <c r="DF53">
-        <v>0</v>
-      </c>
-      <c r="DG53">
-        <v>0</v>
-      </c>
-      <c r="DH53">
-        <v>0</v>
-      </c>
-      <c r="DI53">
-        <v>0</v>
-      </c>
-      <c r="DJ53">
-        <v>0</v>
-      </c>
-      <c r="DK53">
-        <v>0</v>
-      </c>
-      <c r="DL53">
-        <v>0</v>
-      </c>
-      <c r="DM53">
-        <v>0</v>
-      </c>
-      <c r="DN53">
-        <v>0</v>
-      </c>
-      <c r="DO53">
-        <v>0</v>
-      </c>
-      <c r="DP53">
-        <v>0</v>
-      </c>
-      <c r="DQ53">
-        <v>0</v>
-      </c>
-      <c r="DR53">
-        <v>0</v>
-      </c>
-      <c r="DS53">
-        <v>0</v>
-      </c>
-      <c r="DT53">
-        <v>0</v>
-      </c>
-      <c r="DU53">
-        <v>0</v>
-      </c>
-      <c r="DV53">
-        <v>0</v>
-      </c>
-      <c r="DW53">
-        <v>0</v>
-      </c>
-      <c r="DX53">
-        <v>0</v>
-      </c>
-      <c r="DY53">
-        <v>0</v>
-      </c>
-      <c r="DZ53">
-        <v>0</v>
-      </c>
-      <c r="EA53">
-        <v>0</v>
-      </c>
-      <c r="EB53">
-        <v>0</v>
-      </c>
-      <c r="EC53">
-        <v>0</v>
-      </c>
-      <c r="ED53">
-        <v>0</v>
-      </c>
-      <c r="EE53">
-        <v>0</v>
-      </c>
-      <c r="EF53">
-        <v>0</v>
-      </c>
-      <c r="EG53">
-        <v>0</v>
-      </c>
-      <c r="EH53">
-        <v>0</v>
-      </c>
-      <c r="EI53">
-        <v>0</v>
-      </c>
-      <c r="EJ53">
-        <v>0</v>
-      </c>
-      <c r="EK53">
-        <v>0</v>
-      </c>
-      <c r="EL53">
-        <v>0</v>
-      </c>
-      <c r="EM53">
-        <v>0</v>
-      </c>
-      <c r="EN53">
-        <v>0</v>
-      </c>
-      <c r="EO53">
-        <v>-2</v>
-      </c>
-      <c r="EP53">
-        <v>0</v>
-      </c>
-      <c r="EQ53">
-        <v>0</v>
-      </c>
-      <c r="ER53">
-        <v>0</v>
-      </c>
-      <c r="ES53">
-        <v>0</v>
-      </c>
-      <c r="ET53">
-        <v>0</v>
-      </c>
-      <c r="EU53">
-        <v>0</v>
-      </c>
-      <c r="EV53">
-        <v>0</v>
-      </c>
-      <c r="EW53">
-        <v>0</v>
-      </c>
-      <c r="EX53">
-        <v>0</v>
-      </c>
-      <c r="EY53">
-        <v>0</v>
       </c>
       <c r="EZ53">
         <v>0</v>
@@ -41573,7 +41466,7 @@
         <v>0</v>
       </c>
       <c r="W54">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X54">
         <v>0</v>
@@ -41816,160 +41709,160 @@
         <v>0</v>
       </c>
       <c r="CZ54">
+        <v>0</v>
+      </c>
+      <c r="DA54">
+        <v>0</v>
+      </c>
+      <c r="DB54">
+        <v>0</v>
+      </c>
+      <c r="DC54">
+        <v>0</v>
+      </c>
+      <c r="DD54">
+        <v>0</v>
+      </c>
+      <c r="DE54">
+        <v>0</v>
+      </c>
+      <c r="DF54">
+        <v>0</v>
+      </c>
+      <c r="DG54">
+        <v>0</v>
+      </c>
+      <c r="DH54">
+        <v>0</v>
+      </c>
+      <c r="DI54">
+        <v>0</v>
+      </c>
+      <c r="DJ54">
+        <v>-4</v>
+      </c>
+      <c r="DK54">
+        <v>0</v>
+      </c>
+      <c r="DL54">
+        <v>0</v>
+      </c>
+      <c r="DM54">
+        <v>0</v>
+      </c>
+      <c r="DN54">
+        <v>0</v>
+      </c>
+      <c r="DO54">
+        <v>0</v>
+      </c>
+      <c r="DP54">
+        <v>0</v>
+      </c>
+      <c r="DQ54">
+        <v>0</v>
+      </c>
+      <c r="DR54">
+        <v>0</v>
+      </c>
+      <c r="DS54">
+        <v>0</v>
+      </c>
+      <c r="DT54">
+        <v>0</v>
+      </c>
+      <c r="DU54">
+        <v>0</v>
+      </c>
+      <c r="DV54">
+        <v>0</v>
+      </c>
+      <c r="DW54">
+        <v>0</v>
+      </c>
+      <c r="DX54">
+        <v>0</v>
+      </c>
+      <c r="DY54">
+        <v>0</v>
+      </c>
+      <c r="DZ54">
+        <v>0</v>
+      </c>
+      <c r="EA54">
+        <v>0</v>
+      </c>
+      <c r="EB54">
+        <v>0</v>
+      </c>
+      <c r="EC54">
+        <v>0</v>
+      </c>
+      <c r="ED54">
+        <v>0</v>
+      </c>
+      <c r="EE54">
+        <v>0</v>
+      </c>
+      <c r="EF54">
+        <v>0</v>
+      </c>
+      <c r="EG54">
+        <v>0</v>
+      </c>
+      <c r="EH54">
+        <v>0</v>
+      </c>
+      <c r="EI54">
+        <v>0</v>
+      </c>
+      <c r="EJ54">
+        <v>0</v>
+      </c>
+      <c r="EK54">
+        <v>0</v>
+      </c>
+      <c r="EL54">
+        <v>0</v>
+      </c>
+      <c r="EM54">
+        <v>0</v>
+      </c>
+      <c r="EN54">
+        <v>-4</v>
+      </c>
+      <c r="EO54">
+        <v>0</v>
+      </c>
+      <c r="EP54">
+        <v>0</v>
+      </c>
+      <c r="EQ54">
+        <v>0</v>
+      </c>
+      <c r="ER54">
+        <v>0</v>
+      </c>
+      <c r="ES54">
+        <v>0</v>
+      </c>
+      <c r="ET54">
+        <v>0</v>
+      </c>
+      <c r="EU54">
+        <v>0</v>
+      </c>
+      <c r="EV54">
+        <v>0</v>
+      </c>
+      <c r="EW54">
+        <v>0</v>
+      </c>
+      <c r="EX54">
+        <v>0</v>
+      </c>
+      <c r="EY54">
         <v>-2</v>
-      </c>
-      <c r="DA54">
-        <v>0</v>
-      </c>
-      <c r="DB54">
-        <v>0</v>
-      </c>
-      <c r="DC54">
-        <v>0</v>
-      </c>
-      <c r="DD54">
-        <v>0</v>
-      </c>
-      <c r="DE54">
-        <v>0</v>
-      </c>
-      <c r="DF54">
-        <v>0</v>
-      </c>
-      <c r="DG54">
-        <v>0</v>
-      </c>
-      <c r="DH54">
-        <v>0</v>
-      </c>
-      <c r="DI54">
-        <v>0</v>
-      </c>
-      <c r="DJ54">
-        <v>0</v>
-      </c>
-      <c r="DK54">
-        <v>0</v>
-      </c>
-      <c r="DL54">
-        <v>0</v>
-      </c>
-      <c r="DM54">
-        <v>0</v>
-      </c>
-      <c r="DN54">
-        <v>0</v>
-      </c>
-      <c r="DO54">
-        <v>0</v>
-      </c>
-      <c r="DP54">
-        <v>0</v>
-      </c>
-      <c r="DQ54">
-        <v>0</v>
-      </c>
-      <c r="DR54">
-        <v>0</v>
-      </c>
-      <c r="DS54">
-        <v>0</v>
-      </c>
-      <c r="DT54">
-        <v>0</v>
-      </c>
-      <c r="DU54">
-        <v>0</v>
-      </c>
-      <c r="DV54">
-        <v>0</v>
-      </c>
-      <c r="DW54">
-        <v>0</v>
-      </c>
-      <c r="DX54">
-        <v>0</v>
-      </c>
-      <c r="DY54">
-        <v>0</v>
-      </c>
-      <c r="DZ54">
-        <v>0</v>
-      </c>
-      <c r="EA54">
-        <v>0</v>
-      </c>
-      <c r="EB54">
-        <v>0</v>
-      </c>
-      <c r="EC54">
-        <v>0</v>
-      </c>
-      <c r="ED54">
-        <v>0</v>
-      </c>
-      <c r="EE54">
-        <v>0</v>
-      </c>
-      <c r="EF54">
-        <v>0</v>
-      </c>
-      <c r="EG54">
-        <v>0</v>
-      </c>
-      <c r="EH54">
-        <v>0</v>
-      </c>
-      <c r="EI54">
-        <v>0</v>
-      </c>
-      <c r="EJ54">
-        <v>0</v>
-      </c>
-      <c r="EK54">
-        <v>0</v>
-      </c>
-      <c r="EL54">
-        <v>0</v>
-      </c>
-      <c r="EM54">
-        <v>0</v>
-      </c>
-      <c r="EN54">
-        <v>0</v>
-      </c>
-      <c r="EO54">
-        <v>-2</v>
-      </c>
-      <c r="EP54">
-        <v>0</v>
-      </c>
-      <c r="EQ54">
-        <v>0</v>
-      </c>
-      <c r="ER54">
-        <v>0</v>
-      </c>
-      <c r="ES54">
-        <v>0</v>
-      </c>
-      <c r="ET54">
-        <v>0</v>
-      </c>
-      <c r="EU54">
-        <v>0</v>
-      </c>
-      <c r="EV54">
-        <v>0</v>
-      </c>
-      <c r="EW54">
-        <v>0</v>
-      </c>
-      <c r="EX54">
-        <v>0</v>
-      </c>
-      <c r="EY54">
-        <v>0</v>
       </c>
       <c r="EZ54">
         <v>0</v>
@@ -42331,277 +42224,277 @@
         <v>0</v>
       </c>
       <c r="W55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA55">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="AB55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AD55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AE55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AF55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AG55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AH55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AI55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AJ55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AK55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AL55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AM55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AN55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AO55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AP55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AQ55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AR55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AS55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AT55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AU55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AV55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AW55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AX55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AY55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AZ55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BA55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BB55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BC55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BD55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BE55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BF55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BG55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BH55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BI55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BJ55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BK55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BL55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BM55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BN55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BO55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BP55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BQ55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BR55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BS55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BT55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BU55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BV55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BW55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BX55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BY55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BZ55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CA55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CB55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CC55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CD55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CE55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CF55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CG55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CH55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CI55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CJ55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CK55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CL55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CM55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CN55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CO55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CP55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CQ55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CR55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CS55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CT55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CU55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CV55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CW55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CX55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CY55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="CZ55">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="DA55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="DB55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="DC55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="DD55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="DE55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="DF55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="DG55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="DH55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="DI55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="DJ55">
         <v>-1</v>
@@ -42700,34 +42593,34 @@
         <v>-2</v>
       </c>
       <c r="EP55">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="EQ55">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="ER55">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="ES55">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="ET55">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="EU55">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="EV55">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="EW55">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="EX55">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="EY55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="EZ55">
         <v>0</v>
@@ -43332,160 +43225,160 @@
         <v>0</v>
       </c>
       <c r="CZ56">
+        <v>0</v>
+      </c>
+      <c r="DA56">
+        <v>0</v>
+      </c>
+      <c r="DB56">
+        <v>0</v>
+      </c>
+      <c r="DC56">
+        <v>0</v>
+      </c>
+      <c r="DD56">
+        <v>0</v>
+      </c>
+      <c r="DE56">
+        <v>0</v>
+      </c>
+      <c r="DF56">
+        <v>0</v>
+      </c>
+      <c r="DG56">
+        <v>0</v>
+      </c>
+      <c r="DH56">
+        <v>0</v>
+      </c>
+      <c r="DI56">
+        <v>0</v>
+      </c>
+      <c r="DJ56">
+        <v>-4</v>
+      </c>
+      <c r="DK56">
+        <v>0</v>
+      </c>
+      <c r="DL56">
+        <v>0</v>
+      </c>
+      <c r="DM56">
+        <v>0</v>
+      </c>
+      <c r="DN56">
+        <v>0</v>
+      </c>
+      <c r="DO56">
+        <v>0</v>
+      </c>
+      <c r="DP56">
+        <v>0</v>
+      </c>
+      <c r="DQ56">
+        <v>0</v>
+      </c>
+      <c r="DR56">
+        <v>0</v>
+      </c>
+      <c r="DS56">
+        <v>0</v>
+      </c>
+      <c r="DT56">
+        <v>0</v>
+      </c>
+      <c r="DU56">
+        <v>0</v>
+      </c>
+      <c r="DV56">
+        <v>0</v>
+      </c>
+      <c r="DW56">
+        <v>0</v>
+      </c>
+      <c r="DX56">
+        <v>0</v>
+      </c>
+      <c r="DY56">
+        <v>0</v>
+      </c>
+      <c r="DZ56">
+        <v>0</v>
+      </c>
+      <c r="EA56">
+        <v>0</v>
+      </c>
+      <c r="EB56">
+        <v>0</v>
+      </c>
+      <c r="EC56">
+        <v>0</v>
+      </c>
+      <c r="ED56">
+        <v>0</v>
+      </c>
+      <c r="EE56">
+        <v>0</v>
+      </c>
+      <c r="EF56">
+        <v>0</v>
+      </c>
+      <c r="EG56">
+        <v>0</v>
+      </c>
+      <c r="EH56">
+        <v>0</v>
+      </c>
+      <c r="EI56">
+        <v>0</v>
+      </c>
+      <c r="EJ56">
+        <v>0</v>
+      </c>
+      <c r="EK56">
+        <v>0</v>
+      </c>
+      <c r="EL56">
+        <v>0</v>
+      </c>
+      <c r="EM56">
+        <v>0</v>
+      </c>
+      <c r="EN56">
+        <v>-4</v>
+      </c>
+      <c r="EO56">
+        <v>0</v>
+      </c>
+      <c r="EP56">
+        <v>0</v>
+      </c>
+      <c r="EQ56">
+        <v>0</v>
+      </c>
+      <c r="ER56">
+        <v>0</v>
+      </c>
+      <c r="ES56">
+        <v>0</v>
+      </c>
+      <c r="ET56">
+        <v>0</v>
+      </c>
+      <c r="EU56">
+        <v>0</v>
+      </c>
+      <c r="EV56">
+        <v>0</v>
+      </c>
+      <c r="EW56">
+        <v>0</v>
+      </c>
+      <c r="EX56">
+        <v>0</v>
+      </c>
+      <c r="EY56">
         <v>-2</v>
-      </c>
-      <c r="DA56">
-        <v>0</v>
-      </c>
-      <c r="DB56">
-        <v>0</v>
-      </c>
-      <c r="DC56">
-        <v>0</v>
-      </c>
-      <c r="DD56">
-        <v>0</v>
-      </c>
-      <c r="DE56">
-        <v>0</v>
-      </c>
-      <c r="DF56">
-        <v>0</v>
-      </c>
-      <c r="DG56">
-        <v>0</v>
-      </c>
-      <c r="DH56">
-        <v>0</v>
-      </c>
-      <c r="DI56">
-        <v>0</v>
-      </c>
-      <c r="DJ56">
-        <v>0</v>
-      </c>
-      <c r="DK56">
-        <v>0</v>
-      </c>
-      <c r="DL56">
-        <v>0</v>
-      </c>
-      <c r="DM56">
-        <v>0</v>
-      </c>
-      <c r="DN56">
-        <v>0</v>
-      </c>
-      <c r="DO56">
-        <v>0</v>
-      </c>
-      <c r="DP56">
-        <v>0</v>
-      </c>
-      <c r="DQ56">
-        <v>0</v>
-      </c>
-      <c r="DR56">
-        <v>0</v>
-      </c>
-      <c r="DS56">
-        <v>0</v>
-      </c>
-      <c r="DT56">
-        <v>0</v>
-      </c>
-      <c r="DU56">
-        <v>0</v>
-      </c>
-      <c r="DV56">
-        <v>0</v>
-      </c>
-      <c r="DW56">
-        <v>0</v>
-      </c>
-      <c r="DX56">
-        <v>0</v>
-      </c>
-      <c r="DY56">
-        <v>0</v>
-      </c>
-      <c r="DZ56">
-        <v>0</v>
-      </c>
-      <c r="EA56">
-        <v>0</v>
-      </c>
-      <c r="EB56">
-        <v>0</v>
-      </c>
-      <c r="EC56">
-        <v>0</v>
-      </c>
-      <c r="ED56">
-        <v>0</v>
-      </c>
-      <c r="EE56">
-        <v>0</v>
-      </c>
-      <c r="EF56">
-        <v>0</v>
-      </c>
-      <c r="EG56">
-        <v>0</v>
-      </c>
-      <c r="EH56">
-        <v>0</v>
-      </c>
-      <c r="EI56">
-        <v>0</v>
-      </c>
-      <c r="EJ56">
-        <v>0</v>
-      </c>
-      <c r="EK56">
-        <v>0</v>
-      </c>
-      <c r="EL56">
-        <v>0</v>
-      </c>
-      <c r="EM56">
-        <v>0</v>
-      </c>
-      <c r="EN56">
-        <v>0</v>
-      </c>
-      <c r="EO56">
-        <v>-2</v>
-      </c>
-      <c r="EP56">
-        <v>0</v>
-      </c>
-      <c r="EQ56">
-        <v>0</v>
-      </c>
-      <c r="ER56">
-        <v>0</v>
-      </c>
-      <c r="ES56">
-        <v>0</v>
-      </c>
-      <c r="ET56">
-        <v>0</v>
-      </c>
-      <c r="EU56">
-        <v>0</v>
-      </c>
-      <c r="EV56">
-        <v>0</v>
-      </c>
-      <c r="EW56">
-        <v>0</v>
-      </c>
-      <c r="EX56">
-        <v>0</v>
-      </c>
-      <c r="EY56">
-        <v>0</v>
       </c>
       <c r="EZ56">
         <v>0</v>
@@ -44090,160 +43983,160 @@
         <v>0</v>
       </c>
       <c r="CZ57">
+        <v>0</v>
+      </c>
+      <c r="DA57">
+        <v>0</v>
+      </c>
+      <c r="DB57">
+        <v>0</v>
+      </c>
+      <c r="DC57">
+        <v>0</v>
+      </c>
+      <c r="DD57">
+        <v>0</v>
+      </c>
+      <c r="DE57">
+        <v>0</v>
+      </c>
+      <c r="DF57">
+        <v>0</v>
+      </c>
+      <c r="DG57">
+        <v>0</v>
+      </c>
+      <c r="DH57">
+        <v>0</v>
+      </c>
+      <c r="DI57">
+        <v>0</v>
+      </c>
+      <c r="DJ57">
+        <v>-4</v>
+      </c>
+      <c r="DK57">
+        <v>0</v>
+      </c>
+      <c r="DL57">
+        <v>0</v>
+      </c>
+      <c r="DM57">
+        <v>0</v>
+      </c>
+      <c r="DN57">
+        <v>0</v>
+      </c>
+      <c r="DO57">
+        <v>0</v>
+      </c>
+      <c r="DP57">
+        <v>0</v>
+      </c>
+      <c r="DQ57">
+        <v>0</v>
+      </c>
+      <c r="DR57">
+        <v>0</v>
+      </c>
+      <c r="DS57">
+        <v>0</v>
+      </c>
+      <c r="DT57">
+        <v>0</v>
+      </c>
+      <c r="DU57">
+        <v>0</v>
+      </c>
+      <c r="DV57">
+        <v>0</v>
+      </c>
+      <c r="DW57">
+        <v>0</v>
+      </c>
+      <c r="DX57">
+        <v>0</v>
+      </c>
+      <c r="DY57">
+        <v>0</v>
+      </c>
+      <c r="DZ57">
+        <v>0</v>
+      </c>
+      <c r="EA57">
+        <v>0</v>
+      </c>
+      <c r="EB57">
+        <v>0</v>
+      </c>
+      <c r="EC57">
+        <v>0</v>
+      </c>
+      <c r="ED57">
+        <v>0</v>
+      </c>
+      <c r="EE57">
+        <v>0</v>
+      </c>
+      <c r="EF57">
+        <v>0</v>
+      </c>
+      <c r="EG57">
+        <v>0</v>
+      </c>
+      <c r="EH57">
+        <v>0</v>
+      </c>
+      <c r="EI57">
+        <v>0</v>
+      </c>
+      <c r="EJ57">
+        <v>0</v>
+      </c>
+      <c r="EK57">
+        <v>0</v>
+      </c>
+      <c r="EL57">
+        <v>0</v>
+      </c>
+      <c r="EM57">
+        <v>0</v>
+      </c>
+      <c r="EN57">
+        <v>-4</v>
+      </c>
+      <c r="EO57">
+        <v>0</v>
+      </c>
+      <c r="EP57">
+        <v>0</v>
+      </c>
+      <c r="EQ57">
+        <v>0</v>
+      </c>
+      <c r="ER57">
+        <v>0</v>
+      </c>
+      <c r="ES57">
+        <v>0</v>
+      </c>
+      <c r="ET57">
+        <v>0</v>
+      </c>
+      <c r="EU57">
+        <v>0</v>
+      </c>
+      <c r="EV57">
+        <v>0</v>
+      </c>
+      <c r="EW57">
+        <v>0</v>
+      </c>
+      <c r="EX57">
+        <v>0</v>
+      </c>
+      <c r="EY57">
         <v>-2</v>
-      </c>
-      <c r="DA57">
-        <v>0</v>
-      </c>
-      <c r="DB57">
-        <v>0</v>
-      </c>
-      <c r="DC57">
-        <v>0</v>
-      </c>
-      <c r="DD57">
-        <v>0</v>
-      </c>
-      <c r="DE57">
-        <v>0</v>
-      </c>
-      <c r="DF57">
-        <v>0</v>
-      </c>
-      <c r="DG57">
-        <v>0</v>
-      </c>
-      <c r="DH57">
-        <v>0</v>
-      </c>
-      <c r="DI57">
-        <v>0</v>
-      </c>
-      <c r="DJ57">
-        <v>0</v>
-      </c>
-      <c r="DK57">
-        <v>0</v>
-      </c>
-      <c r="DL57">
-        <v>0</v>
-      </c>
-      <c r="DM57">
-        <v>0</v>
-      </c>
-      <c r="DN57">
-        <v>0</v>
-      </c>
-      <c r="DO57">
-        <v>0</v>
-      </c>
-      <c r="DP57">
-        <v>0</v>
-      </c>
-      <c r="DQ57">
-        <v>0</v>
-      </c>
-      <c r="DR57">
-        <v>0</v>
-      </c>
-      <c r="DS57">
-        <v>0</v>
-      </c>
-      <c r="DT57">
-        <v>0</v>
-      </c>
-      <c r="DU57">
-        <v>0</v>
-      </c>
-      <c r="DV57">
-        <v>0</v>
-      </c>
-      <c r="DW57">
-        <v>0</v>
-      </c>
-      <c r="DX57">
-        <v>0</v>
-      </c>
-      <c r="DY57">
-        <v>0</v>
-      </c>
-      <c r="DZ57">
-        <v>0</v>
-      </c>
-      <c r="EA57">
-        <v>0</v>
-      </c>
-      <c r="EB57">
-        <v>0</v>
-      </c>
-      <c r="EC57">
-        <v>0</v>
-      </c>
-      <c r="ED57">
-        <v>0</v>
-      </c>
-      <c r="EE57">
-        <v>0</v>
-      </c>
-      <c r="EF57">
-        <v>0</v>
-      </c>
-      <c r="EG57">
-        <v>0</v>
-      </c>
-      <c r="EH57">
-        <v>0</v>
-      </c>
-      <c r="EI57">
-        <v>0</v>
-      </c>
-      <c r="EJ57">
-        <v>0</v>
-      </c>
-      <c r="EK57">
-        <v>0</v>
-      </c>
-      <c r="EL57">
-        <v>0</v>
-      </c>
-      <c r="EM57">
-        <v>0</v>
-      </c>
-      <c r="EN57">
-        <v>0</v>
-      </c>
-      <c r="EO57">
-        <v>-2</v>
-      </c>
-      <c r="EP57">
-        <v>0</v>
-      </c>
-      <c r="EQ57">
-        <v>0</v>
-      </c>
-      <c r="ER57">
-        <v>0</v>
-      </c>
-      <c r="ES57">
-        <v>0</v>
-      </c>
-      <c r="ET57">
-        <v>0</v>
-      </c>
-      <c r="EU57">
-        <v>0</v>
-      </c>
-      <c r="EV57">
-        <v>0</v>
-      </c>
-      <c r="EW57">
-        <v>0</v>
-      </c>
-      <c r="EX57">
-        <v>0</v>
-      </c>
-      <c r="EY57">
-        <v>0</v>
       </c>
       <c r="EZ57">
         <v>0</v>
@@ -44848,160 +44741,160 @@
         <v>0</v>
       </c>
       <c r="CZ58">
+        <v>0</v>
+      </c>
+      <c r="DA58">
+        <v>0</v>
+      </c>
+      <c r="DB58">
+        <v>0</v>
+      </c>
+      <c r="DC58">
+        <v>0</v>
+      </c>
+      <c r="DD58">
+        <v>0</v>
+      </c>
+      <c r="DE58">
+        <v>0</v>
+      </c>
+      <c r="DF58">
+        <v>0</v>
+      </c>
+      <c r="DG58">
+        <v>0</v>
+      </c>
+      <c r="DH58">
+        <v>0</v>
+      </c>
+      <c r="DI58">
+        <v>0</v>
+      </c>
+      <c r="DJ58">
+        <v>-4</v>
+      </c>
+      <c r="DK58">
+        <v>0</v>
+      </c>
+      <c r="DL58">
+        <v>0</v>
+      </c>
+      <c r="DM58">
+        <v>0</v>
+      </c>
+      <c r="DN58">
+        <v>0</v>
+      </c>
+      <c r="DO58">
+        <v>0</v>
+      </c>
+      <c r="DP58">
+        <v>0</v>
+      </c>
+      <c r="DQ58">
+        <v>0</v>
+      </c>
+      <c r="DR58">
+        <v>0</v>
+      </c>
+      <c r="DS58">
+        <v>0</v>
+      </c>
+      <c r="DT58">
+        <v>0</v>
+      </c>
+      <c r="DU58">
+        <v>0</v>
+      </c>
+      <c r="DV58">
+        <v>0</v>
+      </c>
+      <c r="DW58">
+        <v>0</v>
+      </c>
+      <c r="DX58">
+        <v>0</v>
+      </c>
+      <c r="DY58">
+        <v>0</v>
+      </c>
+      <c r="DZ58">
+        <v>0</v>
+      </c>
+      <c r="EA58">
+        <v>0</v>
+      </c>
+      <c r="EB58">
+        <v>0</v>
+      </c>
+      <c r="EC58">
+        <v>0</v>
+      </c>
+      <c r="ED58">
+        <v>0</v>
+      </c>
+      <c r="EE58">
+        <v>0</v>
+      </c>
+      <c r="EF58">
+        <v>0</v>
+      </c>
+      <c r="EG58">
+        <v>0</v>
+      </c>
+      <c r="EH58">
+        <v>0</v>
+      </c>
+      <c r="EI58">
+        <v>0</v>
+      </c>
+      <c r="EJ58">
+        <v>0</v>
+      </c>
+      <c r="EK58">
+        <v>0</v>
+      </c>
+      <c r="EL58">
+        <v>0</v>
+      </c>
+      <c r="EM58">
+        <v>0</v>
+      </c>
+      <c r="EN58">
+        <v>-4</v>
+      </c>
+      <c r="EO58">
+        <v>0</v>
+      </c>
+      <c r="EP58">
+        <v>0</v>
+      </c>
+      <c r="EQ58">
+        <v>0</v>
+      </c>
+      <c r="ER58">
+        <v>0</v>
+      </c>
+      <c r="ES58">
+        <v>0</v>
+      </c>
+      <c r="ET58">
+        <v>0</v>
+      </c>
+      <c r="EU58">
+        <v>0</v>
+      </c>
+      <c r="EV58">
+        <v>0</v>
+      </c>
+      <c r="EW58">
+        <v>0</v>
+      </c>
+      <c r="EX58">
+        <v>0</v>
+      </c>
+      <c r="EY58">
         <v>-2</v>
-      </c>
-      <c r="DA58">
-        <v>0</v>
-      </c>
-      <c r="DB58">
-        <v>0</v>
-      </c>
-      <c r="DC58">
-        <v>0</v>
-      </c>
-      <c r="DD58">
-        <v>0</v>
-      </c>
-      <c r="DE58">
-        <v>0</v>
-      </c>
-      <c r="DF58">
-        <v>0</v>
-      </c>
-      <c r="DG58">
-        <v>0</v>
-      </c>
-      <c r="DH58">
-        <v>0</v>
-      </c>
-      <c r="DI58">
-        <v>0</v>
-      </c>
-      <c r="DJ58">
-        <v>0</v>
-      </c>
-      <c r="DK58">
-        <v>0</v>
-      </c>
-      <c r="DL58">
-        <v>0</v>
-      </c>
-      <c r="DM58">
-        <v>0</v>
-      </c>
-      <c r="DN58">
-        <v>0</v>
-      </c>
-      <c r="DO58">
-        <v>0</v>
-      </c>
-      <c r="DP58">
-        <v>0</v>
-      </c>
-      <c r="DQ58">
-        <v>0</v>
-      </c>
-      <c r="DR58">
-        <v>0</v>
-      </c>
-      <c r="DS58">
-        <v>0</v>
-      </c>
-      <c r="DT58">
-        <v>0</v>
-      </c>
-      <c r="DU58">
-        <v>0</v>
-      </c>
-      <c r="DV58">
-        <v>0</v>
-      </c>
-      <c r="DW58">
-        <v>0</v>
-      </c>
-      <c r="DX58">
-        <v>0</v>
-      </c>
-      <c r="DY58">
-        <v>0</v>
-      </c>
-      <c r="DZ58">
-        <v>0</v>
-      </c>
-      <c r="EA58">
-        <v>0</v>
-      </c>
-      <c r="EB58">
-        <v>0</v>
-      </c>
-      <c r="EC58">
-        <v>0</v>
-      </c>
-      <c r="ED58">
-        <v>0</v>
-      </c>
-      <c r="EE58">
-        <v>0</v>
-      </c>
-      <c r="EF58">
-        <v>0</v>
-      </c>
-      <c r="EG58">
-        <v>0</v>
-      </c>
-      <c r="EH58">
-        <v>0</v>
-      </c>
-      <c r="EI58">
-        <v>0</v>
-      </c>
-      <c r="EJ58">
-        <v>0</v>
-      </c>
-      <c r="EK58">
-        <v>0</v>
-      </c>
-      <c r="EL58">
-        <v>0</v>
-      </c>
-      <c r="EM58">
-        <v>0</v>
-      </c>
-      <c r="EN58">
-        <v>0</v>
-      </c>
-      <c r="EO58">
-        <v>-2</v>
-      </c>
-      <c r="EP58">
-        <v>0</v>
-      </c>
-      <c r="EQ58">
-        <v>0</v>
-      </c>
-      <c r="ER58">
-        <v>0</v>
-      </c>
-      <c r="ES58">
-        <v>0</v>
-      </c>
-      <c r="ET58">
-        <v>0</v>
-      </c>
-      <c r="EU58">
-        <v>0</v>
-      </c>
-      <c r="EV58">
-        <v>0</v>
-      </c>
-      <c r="EW58">
-        <v>0</v>
-      </c>
-      <c r="EX58">
-        <v>0</v>
-      </c>
-      <c r="EY58">
-        <v>0</v>
       </c>
       <c r="EZ58">
         <v>0</v>
@@ -45729,37 +45622,37 @@
         <v>-1</v>
       </c>
       <c r="EO59">
+        <v>0</v>
+      </c>
+      <c r="EP59">
+        <v>0</v>
+      </c>
+      <c r="EQ59">
+        <v>0</v>
+      </c>
+      <c r="ER59">
+        <v>0</v>
+      </c>
+      <c r="ES59">
+        <v>0</v>
+      </c>
+      <c r="ET59">
+        <v>0</v>
+      </c>
+      <c r="EU59">
+        <v>0</v>
+      </c>
+      <c r="EV59">
+        <v>0</v>
+      </c>
+      <c r="EW59">
+        <v>0</v>
+      </c>
+      <c r="EX59">
+        <v>0</v>
+      </c>
+      <c r="EY59">
         <v>-2</v>
-      </c>
-      <c r="EP59">
-        <v>0</v>
-      </c>
-      <c r="EQ59">
-        <v>0</v>
-      </c>
-      <c r="ER59">
-        <v>0</v>
-      </c>
-      <c r="ES59">
-        <v>0</v>
-      </c>
-      <c r="ET59">
-        <v>0</v>
-      </c>
-      <c r="EU59">
-        <v>0</v>
-      </c>
-      <c r="EV59">
-        <v>0</v>
-      </c>
-      <c r="EW59">
-        <v>0</v>
-      </c>
-      <c r="EX59">
-        <v>0</v>
-      </c>
-      <c r="EY59">
-        <v>0</v>
       </c>
       <c r="EZ59">
         <v>0</v>
@@ -46520,229 +46413,229 @@
         <v>-1</v>
       </c>
       <c r="EZ60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FA60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FB60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FC60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FD60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FE60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FF60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FG60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FH60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FI60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FJ60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FK60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FL60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FM60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FN60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FO60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FP60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FQ60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FR60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FS60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FT60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FU60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FV60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FW60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FX60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FY60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="FZ60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GA60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GB60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GC60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GD60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GE60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GF60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GG60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GH60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GI60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GJ60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GK60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GL60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GM60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GN60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GO60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GP60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GQ60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GR60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GS60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GT60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GU60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GV60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GW60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GX60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GY60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="GZ60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="HA60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="HB60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="HC60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="HD60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="HE60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="HF60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="HG60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="HH60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="HI60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="HJ60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="HK60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="HL60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="HM60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="HN60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="HO60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="HP60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="HQ60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="HR60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="HS60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="HT60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="HU60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="HV60">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="HW60">
         <v>-1</v>
@@ -79407,25 +79300,30 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A104:XFD1048576 A74:Y74 AX74:DL74 A1:XFD73 A75:DL103 DM74:XFD103">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
       <formula>-2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
       <formula>-1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z74:AW74">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>-2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>-1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:IR103">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+      <formula>-4</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>